<commit_message>
ajustando código do T2 para o T3
</commit_message>
<xml_diff>
--- a/Tabela-Sintática-ação-e-desvio.xlsx
+++ b/Tabela-Sintática-ação-e-desvio.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\matheus\google drive\10 período\compiladores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\matheus\documents\github\analisadorlexico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07D50A2-1A1C-4A05-A273-A5689513C21C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCDD792-5A11-417E-A15A-DFD6D2314204}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{743656EB-DE79-4C6B-8F28-BAC11504A692}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{743656EB-DE79-4C6B-8F28-BAC11504A692}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminais" sheetId="1" r:id="rId1"/>
     <sheet name="Não terminais" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="118">
   <si>
     <t>Estados</t>
   </si>
@@ -94,9 +95,6 @@
     <t>varfim</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>real</t>
   </si>
   <si>
@@ -374,6 +372,15 @@
   </si>
   <si>
     <t>ERR</t>
+  </si>
+  <si>
+    <t>S37</t>
+  </si>
+  <si>
+    <t>S38</t>
+  </si>
+  <si>
+    <t>inteiro</t>
   </si>
 </sst>
 </file>
@@ -438,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -447,6 +454,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,11 +769,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB98546E-142E-4D9F-9E9B-17B6E135EF4B}">
-  <dimension ref="A1:Z77"/>
+  <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,70 +792,70 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" t="s">
-        <v>74</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" t="s">
-        <v>40</v>
-      </c>
       <c r="Z1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -855,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -863,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="Z3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -871,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -879,22 +887,22 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" t="s">
         <v>45</v>
-      </c>
-      <c r="I5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>48</v>
-      </c>
-      <c r="N5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P5" t="s">
-        <v>49</v>
-      </c>
-      <c r="R5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -902,16 +910,16 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
         <v>62</v>
-      </c>
-      <c r="G6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -919,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="Z7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -927,22 +935,22 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P8" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" t="s">
         <v>45</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" t="s">
-        <v>47</v>
-      </c>
-      <c r="P8" t="s">
-        <v>49</v>
-      </c>
-      <c r="R8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -950,22 +958,22 @@
         <v>7</v>
       </c>
       <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" t="s">
         <v>45</v>
-      </c>
-      <c r="I9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
@@ -973,22 +981,22 @@
         <v>8</v>
       </c>
       <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" t="s">
         <v>45</v>
-      </c>
-      <c r="I10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N10" t="s">
-        <v>47</v>
-      </c>
-      <c r="P10" t="s">
-        <v>49</v>
-      </c>
-      <c r="R10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
@@ -996,22 +1004,22 @@
         <v>9</v>
       </c>
       <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P11" t="s">
+        <v>48</v>
+      </c>
+      <c r="R11" t="s">
         <v>45</v>
-      </c>
-      <c r="I11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" t="s">
-        <v>47</v>
-      </c>
-      <c r="P11" t="s">
-        <v>49</v>
-      </c>
-      <c r="R11" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
@@ -1019,7 +1027,7 @@
         <v>10</v>
       </c>
       <c r="Z12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
@@ -1027,7 +1035,7 @@
         <v>11</v>
       </c>
       <c r="R13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -1035,13 +1043,13 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q14" t="s">
         <v>55</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>56</v>
-      </c>
-      <c r="R14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -1049,7 +1057,7 @@
         <v>13</v>
       </c>
       <c r="T15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -1057,35 +1065,35 @@
         <v>14</v>
       </c>
       <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" t="s">
         <v>45</v>
-      </c>
-      <c r="I16" t="s">
-        <v>44</v>
-      </c>
-      <c r="K16" t="s">
-        <v>48</v>
-      </c>
-      <c r="M16" t="s">
-        <v>59</v>
-      </c>
-      <c r="R16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="V17">
-        <v>37</v>
+      <c r="V17" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="V18">
-        <v>38</v>
+      <c r="V18" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
@@ -1093,22 +1101,22 @@
         <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -1116,16 +1124,16 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" t="s">
         <v>62</v>
-      </c>
-      <c r="G20" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -1133,7 +1141,7 @@
         <v>19</v>
       </c>
       <c r="X21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
@@ -1141,7 +1149,7 @@
         <v>20</v>
       </c>
       <c r="R22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -1149,10 +1157,10 @@
         <v>21</v>
       </c>
       <c r="X23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Y23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -1160,7 +1168,7 @@
         <v>22</v>
       </c>
       <c r="Z24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
@@ -1168,7 +1176,7 @@
         <v>23</v>
       </c>
       <c r="Z25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -1176,7 +1184,7 @@
         <v>24</v>
       </c>
       <c r="Z26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -1184,7 +1192,7 @@
         <v>25</v>
       </c>
       <c r="Z27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
@@ -1192,7 +1200,7 @@
         <v>26</v>
       </c>
       <c r="X28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -1200,7 +1208,7 @@
         <v>27</v>
       </c>
       <c r="X29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -1208,7 +1216,7 @@
         <v>28</v>
       </c>
       <c r="X30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
@@ -1216,7 +1224,7 @@
         <v>29</v>
       </c>
       <c r="X31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
@@ -1224,7 +1232,7 @@
         <v>30</v>
       </c>
       <c r="X32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.3">
@@ -1232,10 +1240,10 @@
         <v>31</v>
       </c>
       <c r="Q33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
@@ -1243,28 +1251,28 @@
         <v>32</v>
       </c>
       <c r="H34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
@@ -1272,19 +1280,19 @@
         <v>33</v>
       </c>
       <c r="H35" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" t="s">
+        <v>47</v>
+      </c>
+      <c r="M35" t="s">
+        <v>58</v>
+      </c>
+      <c r="R35" t="s">
         <v>45</v>
-      </c>
-      <c r="I35" t="s">
-        <v>44</v>
-      </c>
-      <c r="K35" t="s">
-        <v>48</v>
-      </c>
-      <c r="M35" t="s">
-        <v>59</v>
-      </c>
-      <c r="R35" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
@@ -1292,19 +1300,19 @@
         <v>34</v>
       </c>
       <c r="H36" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K36" t="s">
+        <v>47</v>
+      </c>
+      <c r="M36" t="s">
+        <v>58</v>
+      </c>
+      <c r="R36" t="s">
         <v>45</v>
-      </c>
-      <c r="I36" t="s">
-        <v>44</v>
-      </c>
-      <c r="K36" t="s">
-        <v>48</v>
-      </c>
-      <c r="M36" t="s">
-        <v>59</v>
-      </c>
-      <c r="R36" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
@@ -1312,19 +1320,19 @@
         <v>35</v>
       </c>
       <c r="H37" t="s">
+        <v>44</v>
+      </c>
+      <c r="I37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" t="s">
+        <v>47</v>
+      </c>
+      <c r="M37" t="s">
+        <v>58</v>
+      </c>
+      <c r="R37" t="s">
         <v>45</v>
-      </c>
-      <c r="I37" t="s">
-        <v>44</v>
-      </c>
-      <c r="K37" t="s">
-        <v>48</v>
-      </c>
-      <c r="M37" t="s">
-        <v>59</v>
-      </c>
-      <c r="R37" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
@@ -1332,28 +1340,28 @@
         <v>36</v>
       </c>
       <c r="H38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
@@ -1361,10 +1369,10 @@
         <v>37</v>
       </c>
       <c r="Q39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.3">
@@ -1372,10 +1380,10 @@
         <v>38</v>
       </c>
       <c r="Q40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.3">
@@ -1383,22 +1391,22 @@
         <v>39</v>
       </c>
       <c r="H41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.3">
@@ -1406,22 +1414,22 @@
         <v>40</v>
       </c>
       <c r="H42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.3">
@@ -1429,7 +1437,7 @@
         <v>41</v>
       </c>
       <c r="X43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.3">
@@ -1437,7 +1445,7 @@
         <v>42</v>
       </c>
       <c r="R44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.3">
@@ -1445,7 +1453,7 @@
         <v>43</v>
       </c>
       <c r="R45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.3">
@@ -1453,7 +1461,7 @@
         <v>44</v>
       </c>
       <c r="R46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.3">
@@ -1461,7 +1469,7 @@
         <v>45</v>
       </c>
       <c r="R47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.3">
@@ -1469,28 +1477,28 @@
         <v>46</v>
       </c>
       <c r="H48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.3">
@@ -1498,28 +1506,28 @@
         <v>47</v>
       </c>
       <c r="H49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
@@ -1527,7 +1535,7 @@
         <v>48</v>
       </c>
       <c r="X50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.3">
@@ -1535,10 +1543,10 @@
         <v>49</v>
       </c>
       <c r="U51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.3">
@@ -1546,16 +1554,16 @@
         <v>50</v>
       </c>
       <c r="S52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.3">
@@ -1563,16 +1571,16 @@
         <v>51</v>
       </c>
       <c r="S53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.3">
@@ -1580,28 +1588,28 @@
         <v>52</v>
       </c>
       <c r="H54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.3">
@@ -1609,28 +1617,28 @@
         <v>53</v>
       </c>
       <c r="H55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.3">
@@ -1638,28 +1646,28 @@
         <v>54</v>
       </c>
       <c r="H56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.3">
@@ -1667,7 +1675,7 @@
         <v>55</v>
       </c>
       <c r="W57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.3">
@@ -1675,7 +1683,7 @@
         <v>56</v>
       </c>
       <c r="S58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.3">
@@ -1683,7 +1691,7 @@
         <v>57</v>
       </c>
       <c r="W59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.3">
@@ -1691,16 +1699,16 @@
         <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.3">
@@ -1708,7 +1716,7 @@
         <v>59</v>
       </c>
       <c r="X61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.3">
@@ -1716,28 +1724,28 @@
         <v>60</v>
       </c>
       <c r="H62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.3">
@@ -1745,10 +1753,10 @@
         <v>61</v>
       </c>
       <c r="Q63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.3">
@@ -1756,19 +1764,19 @@
         <v>62</v>
       </c>
       <c r="H64" t="s">
+        <v>44</v>
+      </c>
+      <c r="I64" t="s">
+        <v>43</v>
+      </c>
+      <c r="K64" t="s">
+        <v>47</v>
+      </c>
+      <c r="O64" t="s">
+        <v>75</v>
+      </c>
+      <c r="R64" t="s">
         <v>45</v>
-      </c>
-      <c r="I64" t="s">
-        <v>44</v>
-      </c>
-      <c r="K64" t="s">
-        <v>48</v>
-      </c>
-      <c r="M64" t="s">
-        <v>76</v>
-      </c>
-      <c r="R64" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.3">
@@ -1776,10 +1784,10 @@
         <v>63</v>
       </c>
       <c r="Q65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.3">
@@ -1787,15 +1795,16 @@
         <v>64</v>
       </c>
       <c r="L66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
+      <c r="H67" s="4"/>
       <c r="X67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.3">
@@ -1803,22 +1812,22 @@
         <v>66</v>
       </c>
       <c r="H68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.3">
@@ -1826,19 +1835,19 @@
         <v>67</v>
       </c>
       <c r="H69" t="s">
+        <v>44</v>
+      </c>
+      <c r="I69" t="s">
+        <v>43</v>
+      </c>
+      <c r="K69" t="s">
+        <v>47</v>
+      </c>
+      <c r="O69" t="s">
+        <v>75</v>
+      </c>
+      <c r="R69" t="s">
         <v>45</v>
-      </c>
-      <c r="I69" t="s">
-        <v>44</v>
-      </c>
-      <c r="K69" t="s">
-        <v>48</v>
-      </c>
-      <c r="M69" t="s">
-        <v>76</v>
-      </c>
-      <c r="R69" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.3">
@@ -1846,19 +1855,19 @@
         <v>68</v>
       </c>
       <c r="H70" t="s">
+        <v>44</v>
+      </c>
+      <c r="I70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K70" t="s">
+        <v>47</v>
+      </c>
+      <c r="O70" t="s">
+        <v>75</v>
+      </c>
+      <c r="R70" t="s">
         <v>45</v>
-      </c>
-      <c r="I70" t="s">
-        <v>44</v>
-      </c>
-      <c r="K70" t="s">
-        <v>48</v>
-      </c>
-      <c r="M70" t="s">
-        <v>76</v>
-      </c>
-      <c r="R70" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.3">
@@ -1866,19 +1875,19 @@
         <v>69</v>
       </c>
       <c r="H71" t="s">
+        <v>44</v>
+      </c>
+      <c r="I71" t="s">
+        <v>43</v>
+      </c>
+      <c r="K71" t="s">
+        <v>47</v>
+      </c>
+      <c r="O71" t="s">
+        <v>75</v>
+      </c>
+      <c r="R71" t="s">
         <v>45</v>
-      </c>
-      <c r="I71" t="s">
-        <v>44</v>
-      </c>
-      <c r="K71" t="s">
-        <v>48</v>
-      </c>
-      <c r="M71" t="s">
-        <v>76</v>
-      </c>
-      <c r="R71" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.3">
@@ -1886,124 +1895,133 @@
         <v>70</v>
       </c>
       <c r="H72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
+      <c r="G73" s="4"/>
       <c r="W73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
+      <c r="G74" s="4"/>
       <c r="H74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
+      <c r="G75" s="4"/>
       <c r="H75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
+      <c r="G76" s="4"/>
       <c r="H76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
+      <c r="G77" s="4"/>
       <c r="H77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R77" t="s">
-        <v>114</v>
-      </c>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G78" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2011,9 +2029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838FF180-2F18-4F46-AEFC-A5D6131F5028}">
   <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,7 +2104,7 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2159,7 +2177,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>

</xml_diff>